<commit_message>
added PPSS name to district list
</commit_message>
<xml_diff>
--- a/at-regional.xlsx
+++ b/at-regional.xlsx
@@ -413,10 +413,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -551,10 +551,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -685,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -735,13 +735,13 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -860,10 +860,10 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -985,10 +985,10 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1035,13 +1035,13 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizado con procesa de carga de AT cunamas
</commit_message>
<xml_diff>
--- a/at-regional.xlsx
+++ b/at-regional.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,60 +365,105 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>AT_ETR_052022</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AT_ETL_052022</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>AT_GORE_052022</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>AT_ETR_062022</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>AT_ETL_062022</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>AT_GORE_062022</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>AT_ETR_072022</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>AT_ETL_072022</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>AT_GORE_072022</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>AT_ETR_082022</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>AT_ETL_082022</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>AT_GORE_082022</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>AT_ETR_092022</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>AT_ETL_092022</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>AT_GORE_092022</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>AT_ETR_102022</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>AT_ETL_102022</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>AT_GORE_102022</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>AT_ETR_112022</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>AT_ETL_112022</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>AT_GORE_112022</t>
         </is>
@@ -443,27 +488,54 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
         <v>4</v>
       </c>
-      <c r="J2">
+      <c r="S2">
         <v>3</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
         <v>0</v>
       </c>
     </row>
@@ -474,39 +546,66 @@
         </is>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <v>3</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
         <v>1</v>
       </c>
     </row>
@@ -517,7 +616,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -526,31 +625,58 @@
         <v>0</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -560,40 +686,67 @@
         </is>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>3</v>
       </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -612,22 +765,22 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -636,6 +789,33 @@
         <v>0</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
         <v>0</v>
       </c>
     </row>
@@ -646,39 +826,66 @@
         </is>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
         <v>6</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
         <v>3</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="V7">
         <v>0</v>
       </c>
     </row>
@@ -716,13 +923,40 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -732,28 +966,28 @@
         </is>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -765,6 +999,33 @@
         <v>0</v>
       </c>
       <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
         <v>0</v>
       </c>
     </row>
@@ -775,39 +1036,66 @@
         </is>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
         <v>4</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
         <v>0</v>
       </c>
     </row>
@@ -827,31 +1115,58 @@
         <v>0</v>
       </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <v>3</v>
       </c>
-      <c r="F11">
+      <c r="O11">
         <v>5</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>2</v>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -861,39 +1176,66 @@
         </is>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>2</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
         <v>1</v>
       </c>
     </row>
@@ -913,30 +1255,57 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
         <v>5</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
         <v>1</v>
       </c>
     </row>
@@ -947,31 +1316,31 @@
         </is>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -980,6 +1349,33 @@
         <v>1</v>
       </c>
       <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
         <v>1</v>
       </c>
     </row>
@@ -990,31 +1386,31 @@
         </is>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1023,7 +1419,34 @@
         <v>2</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1066,6 +1489,33 @@
         <v>0</v>
       </c>
       <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>2</v>
+      </c>
+      <c r="V16">
         <v>1</v>
       </c>
     </row>
@@ -1082,16 +1532,16 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1109,6 +1559,33 @@
         <v>0</v>
       </c>
       <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>0</v>
       </c>
     </row>
@@ -1122,37 +1599,64 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
         <v>8</v>
       </c>
-      <c r="J18">
-        <v>2</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
+      <c r="S18">
+        <v>2</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>8</v>
+      </c>
+      <c r="V18">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1162,39 +1666,66 @@
         </is>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
         <v>3</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
         <v>3</v>
       </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
         <v>0</v>
       </c>
     </row>
@@ -1205,7 +1736,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1214,31 +1745,58 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <v>0</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1251,37 +1809,64 @@
         <v>0</v>
       </c>
       <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
         <v>3</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
       <c r="M21">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1294,36 +1879,63 @@
         <v>0</v>
       </c>
       <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
         <v>4</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
         <v>4</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
         <v>3</v>
       </c>
-      <c r="J22">
-        <v>2</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22">
+      <c r="S22">
+        <v>2</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
         <v>0</v>
       </c>
     </row>
@@ -1343,30 +1955,57 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>2</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
         <v>0</v>
       </c>
     </row>
@@ -1377,7 +2016,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1386,30 +2025,57 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>3</v>
+      </c>
+      <c r="V24">
         <v>0</v>
       </c>
     </row>
@@ -1420,39 +2086,66 @@
         </is>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>2</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25">
         <v>1</v>
       </c>
     </row>
@@ -1466,36 +2159,63 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <v>2</v>
       </c>
       <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>2</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>2</v>
+      </c>
+      <c r="V26">
         <v>1</v>
       </c>
     </row>
@@ -1506,39 +2226,66 @@
         </is>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
         <v>3</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="J27">
-        <v>2</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
       <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>2</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
         <v>0</v>
       </c>
     </row>

</xml_diff>